<commit_message>
🤖 Auto scrape: 2025-11-19 04:52:07
</commit_message>
<xml_diff>
--- a/data/11_19_25_tradewheel_scrap.xlsx
+++ b/data/11_19_25_tradewheel_scrap.xlsx
@@ -434,7 +434,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
@@ -477,640 +477,640 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Need prices for charger</t>
+          <t>Searching For Barley</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-prices-for-charger/902386/</t>
+          <t>https://www.tradewheel.com/buyers/searching-for-barley/902128/</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>I am looking for the 100 pcs of chargers that have 3 different ends on one cord. Type C, Iphone , things like that. I am a resaler trying to get a business up and running so looking for just about anything</t>
+          <t>Hello We are looking for Barley in Morocco Our requirement is 300MT please share your good prices Thank you</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Need to Purchase Makeup brushes, Wholesale in bulk</t>
+          <t>Need travel pillow for distribution</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-to-purchase-makeup-brushes-wholesale-in-bulk/902383/</t>
+          <t>https://www.tradewheel.com/buyers/need-travel-pillow-for-distribution/902126/</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Hi I am looking to purchase high-quality vegan makeup brushes, eyeshadow palettes, and beauty sponges. I am also interested in exploring custom-branded options and reviewing your available models to select the most suitable products for my brand....</t>
+          <t>Good day, I want to purchase travel pillow in various material and colors. Please provide me with your available colors, material and shipping charges.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Sri Lanka</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Importing bottle – Need quotes</t>
+          <t>In search of doors for large scale purchase</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/importing-bottle-need-quotes/902374/</t>
+          <t>https://www.tradewheel.com/buyers/in-search-of-doors-for-large-scale-purchase/902123/</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Good day, We would like to purchase water bottles for school and offices use. Hoping to connect soon and explore cooperation opportunities.</t>
+          <t>Hello, I am interested to purchase suitable for residential and commercial use. Kindly share your best offer at your earliest convenience.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Procuring Float Glass for Building and Interior Projects</t>
+          <t>I want to purchase laptops  - Reach me now</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/procuring-float-glass-for-building-and-interior-projects/902372/</t>
+          <t>https://www.tradewheel.com/buyers/i-want-to-purchase-laptops-reach/902118/</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>I want to procure low iron float glass. Thickness: 10 mm Size: 1500 mm x 600 mm Quantity: 4 sheets Delivery to: Singapore Please provide FOB/CIF price and lead time</t>
+          <t>Greetings, Dear Supplier, We require high performance laptops with updated CPUs, SSD storage, and reliable battery life. Please provide detailed, warranty terms, and certification information.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Buying sugar for export.</t>
+          <t>Inquiry about: All Ages Soccer Sneakers Firm Soft Ground Outdoor Indoor Men Football Cleats Cheap Turf Soccer Shoes</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/buying-sugar-for-export/902371/</t>
+          <t>https://www.tradewheel.com/buyers/inquiry-about-all-ages-soccer-sneakers-firm-soft/902116/</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Greetings, We require bulk quantities of sugar at wholesale price. Kindly share your catalog, minimum order quantity along with delivery timeline.</t>
+          <t>hello I am very interested in your soccer cleats. Do you dropship?</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sourcing Hair Treatment Products for Salon and Retail Use</t>
+          <t>Looking to purchase skin care accessories</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/sourcing-hair-treatment-products-for-salon-and-retail/902370/</t>
+          <t>https://www.tradewheel.com/buyers/looking-to-purchase-skin-care-accessories/902115/</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>We are purchasing hair treatment products for salons. Types: oils, serums, masks Packaging: bottles, tubes MOQ: 500 units per SKU</t>
+          <t>Dear supplier. I am searching reliable supplier for skin care accessories such as moisturizer, face oil, and cleanser. If there is any supplier who can provide ma at competitive price so contact me via email.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>22 hours ago</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Buying Dump Truck for Heavy-Duty Transport and Logistics</t>
+          <t>Urgent need for video game consoles</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/buying-dump-truck-for-heavy-duty-transport-and-logistics/902369/</t>
+          <t>https://www.tradewheel.com/buyers/urgent-need-for-video-game-consoles/902114/</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>We need 2 units of dump trucks, heavy-duty, suitable for construction sites. Please send full specifications and quotation for review.</t>
+          <t>Hello, We need video game consoles for continuous supply to online and offline markets. Kindly share monthly stock capacity, packaging details, and competitive wholesale rates.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Procuring Car Radio for Automotive Aftermarket Supply</t>
+          <t>Blankets needed for retail chain supply</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/procuring-car-radio-for-automotive-aftermarket-supply/902368/</t>
+          <t>https://www.tradewheel.com/buyers/blankets-needed-for-retail-chain-supply/902112/</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>I’m looking for car radios, 50 pcs, Bluetooth-enabled, FM/AM, suitable for standard dashboards. Please respond with your quotation and lead time.</t>
+          <t>Good day, We want to purchase blankets and need in different material and colors. Please provide material types, available sizes, colors and delivery timeline.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>India</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Need Korean Skincare for Cosmetic Retail Distribution</t>
+          <t>I want to purchase essential oil - Reach me now</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-korean-skincare-for-cosmetic-retail-distribution/902367/</t>
+          <t>https://www.tradewheel.com/buyers/i-want-to-purchase-essential-oil-reach/902111/</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>I’m searching Korean skincare products, 500 units, hydrating and anti-aging formulations, ready for retail packaging. Awaiting your commercial offer for evaluation.</t>
+          <t>Hello, We need essential Oil suitable for food processing. Please send details on shelf life, color, flavor profile, and compliance with international standards.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Zambia</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Buying Electric Heaters for Seasonal Stock and Retail Supply</t>
+          <t>Importing sesame oil – Need quotes</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/buying-electric-heaters-for-seasonal-stock-and-retail/902366/</t>
+          <t>https://www.tradewheel.com/buyers/importing-sesame-oil-need-quotes/902109/</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>I want to source electric heaters in bulk. Features: overheat protection, thermostat Packaging: retail box or bulk Delivery: FOB/CIF</t>
+          <t>Greetings, I want to purchase sesame oil for commercial use and retail purpose. Please send full specifications and quotation for review.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Importing Construction Machinery Parts for Equipment Maintenance</t>
+          <t>Sourcing cocoa beans at competitive price</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/importing-construction-machinery-parts-for-equipment-maintenance/902364/</t>
+          <t>https://www.tradewheel.com/buyers/sourcing-cocoa-beans-at-competitive-price/902106/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>We need 150 units of construction machinery parts, precision-made and durable, suitable for repair and assembly. Awaiting your commercial offer for evaluation.</t>
+          <t>Good day, I am checking availability for cocoa beans and I need 300 ton for the first trial. Kindly share your catalog, MOQ and pricing for large scale purchase. Thank you.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Procuring Dining Table for Home and Office Furniture Supply</t>
+          <t>RFQ for Flat-type dishwasher</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/procuring-dining-table-for-home-and-office-furniture/902363/</t>
+          <t>https://www.tradewheel.com/buyers/rfq-for-flat-type-dishwasher/902104/</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>We require dining tables for wholesale furniture supply. Material: solid wood, engineered wood, glass top Design: modern, classic Size: 120–200 cm length MOQ: 50 pcs</t>
+          <t>I'm looking for Modern Commercial hotel canteen cup washing machine cover-type dishwasher Stainless steel fully automatic dishwashing. Product specifications: ·application: Hotel ·power (w): 9800 ·power source: Electric ·Material: Stainless S...</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sourcing CPUs for Computer Assembly and IT Upgrades</t>
+          <t>Tie down straps wanted for long-term purchase</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/sourcing-cpus-for-computer-assembly-and-it-upgrades/902362/</t>
+          <t>https://www.tradewheel.com/buyers/tie-down-straps-wanted-for-long-term-purchase/902099/</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>We are purchasing CPUs for computer assembly. Type: Intel i5/i7, AMD Ryzen 5/7 Clock speed: 2.5–4.5 GHz Warranty: 1 year MOQ: 50 pcs</t>
+          <t>Hello, We are currently sourcing tie down straps. Our requirements include strong breaking strength, weather resistance and long-lasting performance.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Looking to partner with baby food supplier</t>
+          <t>Need pet products for retail shop</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/looking-to-partner-with-baby-food-supplier/902361/</t>
+          <t>https://www.tradewheel.com/buyers/need-pet-products-for-retail-shop/902095/</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Good day, We are currently sourcing baby food. The products must be made from high-quality ingredients with no harmful additives.</t>
+          <t>Good day, We are interested in buying pet toys and pet products. Interested suppliers may send quotations and available product lines.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Buying Steel Round Bars for Construction and Fabrication Projects</t>
+          <t>Require oxygen sensors with custom specs</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/buying-steel-round-bars-for-construction-and-fabrication/902360/</t>
+          <t>https://www.tradewheel.com/buyers/require-oxygen-sensors-with-custom-specs/902094/</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>I am looking for suppliers of steel round bars. Surface: hot-rolled, cold-rolled Grade: ASTM A36, AISI 304 Packaging: bundled or palletized</t>
+          <t>Good day, We are currently seeking oxygen sensors. The sensors must offer rapid response, long service life and reliable signal output.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Honey needed for retain chain supply</t>
+          <t>I want to buy instant boba tea - reach me now</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/honey-needed-for-retain-chain-supply/902359/</t>
+          <t>https://www.tradewheel.com/buyers/i-want-to-buy-instant-boba-tea/902093/</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Good day, We are interested in buying honey. Could you provide us with availability along with pricing? Kind Regards.</t>
+          <t>Good day, I am interested in buying instant boba tea. Please send product specs, price lists and sample availability. Kind Regards.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Required dried seafood in bulk quantities</t>
+          <t>Searching For Freight Forward Agent</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/required-dried-seafood-in-bulk-quantities/902357/</t>
+          <t>https://www.tradewheel.com/buyers/searching-for-freight-forward-agent/902090/</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Hello, We want to purchase dried seafood suitable for retail sale and food processing. You can reach me through email for quick communication.</t>
+          <t>Hi We are looking forward to move 30kg of books Cairo to Singapore Please share your company details Thanks</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bulk purchase inquiry for plastic cups</t>
+          <t>Need skin care products for distribution</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/bulk-purchase-inquiry-for-plastic-cups/902356/</t>
+          <t>https://www.tradewheel.com/buyers/need-skin-care-products-for-distribution/902088/</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Hello, We are currently seeking plastic cups. We prefer suppliers offering custom printing and eco-friendly options. Kind Regards.</t>
+          <t>Hi there, We are looking for skin care and korean cosmetics. Our preference is for products that emphasize skin hydration, brightening effects and gentle formulations.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>India</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Need cookware sets for distribution</t>
+          <t>Sourcing neodymium magnets at competitive prices</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-cookware-sets-for-distribution/902355/</t>
+          <t>https://www.tradewheel.com/buyers/sourcing-neodymium-magnets-at-competitive-prices/902087/</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Greetings, We are interested in buying cookware sets. The sets must include durable materials, even heat distribution &amp; stainless-steel surfaces.</t>
+          <t>Hello, We are currently sourcing neodymium magnets (NdFeB). The products must offer powerful magnetic force, excellent temperature stability &amp; corrosion resistance.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>15 hours ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Urgent required for phone accessories</t>
+          <t>Require PVC tarps with custom specs</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/urgent-required-for-phone-accessories/902353/</t>
+          <t>https://www.tradewheel.com/buyers/require-pvc-tarps-with-custom-specs/902086/</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>I am interested in future supply options for mobile accessories such as charger, back cover and protector. Contact me through email for specifications and discussion.</t>
+          <t>Hello, We are sourcing PVC tarps and tarpaulin rolls. The products must withstand heavy stretching and exposure to sunlight. Kind Regards.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-11-19 10:03:27</t>
+          <t>2025-11-19 11:24:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 Auto scrape: 2025-11-19 07:16:22
</commit_message>
<xml_diff>
--- a/data/11_19_25_tradewheel_scrap.xlsx
+++ b/data/11_19_25_tradewheel_scrap.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -434,8 +434,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
@@ -477,640 +477,704 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>31 minutes ago</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Searching For Barley</t>
+          <t>Prices For Soybean and Corn</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/searching-for-barley/902128/</t>
+          <t>https://www.tradewheel.com/buyers/prices-for-soybean-and-corn/902542/</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hello We are looking for Barley in Morocco Our requirement is 300MT please share your good prices Thank you</t>
+          <t>Hello We are looking for Soybean and Corn in UK We need about 50MT both Soybean and Corn Kindly share your complete company profile Thank you</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>18 hours ago</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Need travel pillow for distribution</t>
+          <t>Need prices for charger</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-travel-pillow-for-distribution/902126/</t>
+          <t>https://www.tradewheel.com/buyers/need-prices-for-charger/902386/</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Good day, I want to purchase travel pillow in various material and colors. Please provide me with your available colors, material and shipping charges.</t>
+          <t>I am looking for the 100 pcs of chargers that have 3 different ends on one cord. Type C, Iphone , things like that. I am a resaler trying to get a business up and running so looking for just about anything</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sri Lanka</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>18 hours ago</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>In search of doors for large scale purchase</t>
+          <t>Need to Purchase Makeup brushes, Wholesale in bulk</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/in-search-of-doors-for-large-scale-purchase/902123/</t>
+          <t>https://www.tradewheel.com/buyers/need-to-purchase-makeup-brushes-wholesale-in-bulk/902383/</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Hello, I am interested to purchase suitable for residential and commercial use. Kindly share your best offer at your earliest convenience.</t>
+          <t>Hi I am looking to purchase high-quality vegan makeup brushes, eyeshadow palettes, and beauty sponges. I am also interested in exploring custom-branded options and reviewing your available models to select the most suitable products for my brand....</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>I want to purchase laptops  - Reach me now</t>
+          <t>Importing bottle – Need quotes</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/i-want-to-purchase-laptops-reach/902118/</t>
+          <t>https://www.tradewheel.com/buyers/importing-bottle-need-quotes/902374/</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Greetings, Dear Supplier, We require high performance laptops with updated CPUs, SSD storage, and reliable battery life. Please provide detailed, warranty terms, and certification information.</t>
+          <t>Good day, We would like to purchase water bottles for school and offices use. Hoping to connect soon and explore cooperation opportunities.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Inquiry about: All Ages Soccer Sneakers Firm Soft Ground Outdoor Indoor Men Football Cleats Cheap Turf Soccer Shoes</t>
+          <t>Procuring Float Glass for Building and Interior Projects</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/inquiry-about-all-ages-soccer-sneakers-firm-soft/902116/</t>
+          <t>https://www.tradewheel.com/buyers/procuring-float-glass-for-building-and-interior-projects/902372/</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>hello I am very interested in your soccer cleats. Do you dropship?</t>
+          <t>I want to procure low iron float glass. Thickness: 10 mm Size: 1500 mm x 600 mm Quantity: 4 sheets Delivery to: Singapore Please provide FOB/CIF price and lead time</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Looking to purchase skin care accessories</t>
+          <t>Buying sugar for export.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/looking-to-purchase-skin-care-accessories/902115/</t>
+          <t>https://www.tradewheel.com/buyers/buying-sugar-for-export/902371/</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dear supplier. I am searching reliable supplier for skin care accessories such as moisturizer, face oil, and cleanser. If there is any supplier who can provide ma at competitive price so contact me via email.</t>
+          <t>Greetings, We require bulk quantities of sugar at wholesale price. Kindly share your catalog, minimum order quantity along with delivery timeline.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Urgent need for video game consoles</t>
+          <t>Sourcing Hair Treatment Products for Salon and Retail Use</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/urgent-need-for-video-game-consoles/902114/</t>
+          <t>https://www.tradewheel.com/buyers/sourcing-hair-treatment-products-for-salon-and-retail/902370/</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Hello, We need video game consoles for continuous supply to online and offline markets. Kindly share monthly stock capacity, packaging details, and competitive wholesale rates.</t>
+          <t>We are purchasing hair treatment products for salons. Types: oils, serums, masks Packaging: bottles, tubes MOQ: 500 units per SKU</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Blankets needed for retail chain supply</t>
+          <t>Buying Dump Truck for Heavy-Duty Transport and Logistics</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/blankets-needed-for-retail-chain-supply/902112/</t>
+          <t>https://www.tradewheel.com/buyers/buying-dump-truck-for-heavy-duty-transport-and-logistics/902369/</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Good day, We want to purchase blankets and need in different material and colors. Please provide material types, available sizes, colors and delivery timeline.</t>
+          <t>We need 2 units of dump trucks, heavy-duty, suitable for construction sites. Please send full specifications and quotation for review.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>I want to purchase essential oil - Reach me now</t>
+          <t>Procuring Car Radio for Automotive Aftermarket Supply</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/i-want-to-purchase-essential-oil-reach/902111/</t>
+          <t>https://www.tradewheel.com/buyers/procuring-car-radio-for-automotive-aftermarket-supply/902368/</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Hello, We need essential Oil suitable for food processing. Please send details on shelf life, color, flavor profile, and compliance with international standards.</t>
+          <t>I’m looking for car radios, 50 pcs, Bluetooth-enabled, FM/AM, suitable for standard dashboards. Please respond with your quotation and lead time.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Importing sesame oil – Need quotes</t>
+          <t>Need Korean Skincare for Cosmetic Retail Distribution</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/importing-sesame-oil-need-quotes/902109/</t>
+          <t>https://www.tradewheel.com/buyers/need-korean-skincare-for-cosmetic-retail-distribution/902367/</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Greetings, I want to purchase sesame oil for commercial use and retail purpose. Please send full specifications and quotation for review.</t>
+          <t>I’m searching Korean skincare products, 500 units, hydrating and anti-aging formulations, ready for retail packaging. Awaiting your commercial offer for evaluation.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Zambia</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sourcing cocoa beans at competitive price</t>
+          <t>Buying Electric Heaters for Seasonal Stock and Retail Supply</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/sourcing-cocoa-beans-at-competitive-price/902106/</t>
+          <t>https://www.tradewheel.com/buyers/buying-electric-heaters-for-seasonal-stock-and-retail/902366/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Good day, I am checking availability for cocoa beans and I need 300 ton for the first trial. Kindly share your catalog, MOQ and pricing for large scale purchase. Thank you.</t>
+          <t>I want to source electric heaters in bulk. Features: overheat protection, thermostat Packaging: retail box or bulk Delivery: FOB/CIF</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RFQ for Flat-type dishwasher</t>
+          <t>Importing Construction Machinery Parts for Equipment Maintenance</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/rfq-for-flat-type-dishwasher/902104/</t>
+          <t>https://www.tradewheel.com/buyers/importing-construction-machinery-parts-for-equipment-maintenance/902364/</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>I'm looking for Modern Commercial hotel canteen cup washing machine cover-type dishwasher Stainless steel fully automatic dishwashing. Product specifications: ·application: Hotel ·power (w): 9800 ·power source: Electric ·Material: Stainless S...</t>
+          <t>We need 150 units of construction machinery parts, precision-made and durable, suitable for repair and assembly. Awaiting your commercial offer for evaluation.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Tie down straps wanted for long-term purchase</t>
+          <t>Procuring Dining Table for Home and Office Furniture Supply</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/tie-down-straps-wanted-for-long-term-purchase/902099/</t>
+          <t>https://www.tradewheel.com/buyers/procuring-dining-table-for-home-and-office-furniture/902363/</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Hello, We are currently sourcing tie down straps. Our requirements include strong breaking strength, weather resistance and long-lasting performance.</t>
+          <t>We require dining tables for wholesale furniture supply. Material: solid wood, engineered wood, glass top Design: modern, classic Size: 120–200 cm length MOQ: 50 pcs</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Need pet products for retail shop</t>
+          <t>Sourcing CPUs for Computer Assembly and IT Upgrades</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-pet-products-for-retail-shop/902095/</t>
+          <t>https://www.tradewheel.com/buyers/sourcing-cpus-for-computer-assembly-and-it-upgrades/902362/</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Good day, We are interested in buying pet toys and pet products. Interested suppliers may send quotations and available product lines.</t>
+          <t>We are purchasing CPUs for computer assembly. Type: Intel i5/i7, AMD Ryzen 5/7 Clock speed: 2.5–4.5 GHz Warranty: 1 year MOQ: 50 pcs</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Require oxygen sensors with custom specs</t>
+          <t>Looking to partner with baby food supplier</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/require-oxygen-sensors-with-custom-specs/902094/</t>
+          <t>https://www.tradewheel.com/buyers/looking-to-partner-with-baby-food-supplier/902361/</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Good day, We are currently seeking oxygen sensors. The sensors must offer rapid response, long service life and reliable signal output.</t>
+          <t>Good day, We are currently sourcing baby food. The products must be made from high-quality ingredients with no harmful additives.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Hong Kong</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>I want to buy instant boba tea - reach me now</t>
+          <t>Buying Steel Round Bars for Construction and Fabrication Projects</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/i-want-to-buy-instant-boba-tea/902093/</t>
+          <t>https://www.tradewheel.com/buyers/buying-steel-round-bars-for-construction-and-fabrication/902360/</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Good day, I am interested in buying instant boba tea. Please send product specs, price lists and sample availability. Kind Regards.</t>
+          <t>I am looking for suppliers of steel round bars. Surface: hot-rolled, cold-rolled Grade: ASTM A36, AISI 304 Packaging: bundled or palletized</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Searching For Freight Forward Agent</t>
+          <t>Honey needed for retain chain supply</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/searching-for-freight-forward-agent/902090/</t>
+          <t>https://www.tradewheel.com/buyers/honey-needed-for-retain-chain-supply/902359/</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Hi We are looking forward to move 30kg of books Cairo to Singapore Please share your company details Thanks</t>
+          <t>Good day, We are interested in buying honey. Could you provide us with availability along with pricing? Kind Regards.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Hong Kong</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Need skin care products for distribution</t>
+          <t>Required dried seafood in bulk quantities</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/need-skin-care-products-for-distribution/902088/</t>
+          <t>https://www.tradewheel.com/buyers/required-dried-seafood-in-bulk-quantities/902357/</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Hi there, We are looking for skin care and korean cosmetics. Our preference is for products that emphasize skin hydration, brightening effects and gentle formulations.</t>
+          <t>Hello, We want to purchase dried seafood suitable for retail sale and food processing. You can reach me through email for quick communication.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Hong Kong</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1 day ago</t>
+          <t>19 hours ago</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sourcing neodymium magnets at competitive prices</t>
+          <t>Bulk purchase inquiry for plastic cups</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.tradewheel.com/buyers/sourcing-neodymium-magnets-at-competitive-prices/902087/</t>
+          <t>https://www.tradewheel.com/buyers/bulk-purchase-inquiry-for-plastic-cups/902356/</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Hello, We are currently sourcing neodymium magnets (NdFeB). The products must offer powerful magnetic force, excellent temperature stability &amp; corrosion resistance.</t>
+          <t>Hello, We are currently seeking plastic cups. We prefer suppliers offering custom printing and eco-friendly options. Kind Regards.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-11-19 11:24:29</t>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>19 hours ago</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Need cookware sets for distribution</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://www.tradewheel.com/buyers/need-cookware-sets-for-distribution/902355/</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Greetings, We are interested in buying cookware sets. The sets must include durable materials, even heat distribution &amp; stainless-steel surfaces.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-11-19 13:48:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>1 day ago</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Require PVC tarps with custom specs</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>https://www.tradewheel.com/buyers/require-pvc-tarps-with-custom-specs/902086/</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Hello, We are sourcing PVC tarps and tarpaulin rolls. The products must withstand heavy stretching and exposure to sunlight. Kind Regards.</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-11-19 11:24:29</t>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Importing Car Refrigerators – Need Quotes</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://www.tradewheel.com/buyers/importing-car-refrigerators-need-quotes/902134/</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Hello, We would like to purchase Car Refrigerators. We require units with fast cooling, low power consumption and stable performance.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-11-19 13:48:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Buying Telecentric Lens for High-Accuracy Industrial Imaging Projects</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://www.tradewheel.com/buyers/buying-telecentric-lens-for-high-accuracy-industrial-imaging-projects/902133/</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>We require telecentric lens options with low distortion and adjustable working distance for precision measurement tasks. Please respond with your quotation and lead time.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-11-19 13:48:48</t>
         </is>
       </c>
     </row>

</xml_diff>